<commit_message>
Github security findings (#46)
* fixes

* Update: Folium use SVG instead of awesome-markers

* Update: Example output
data

* Fix: Upploaded GPX-Track persists after reload page

---------

Co-authored-by: Rik <rik,mueller@gmail.com>
</commit_message>
<xml_diff>
--- a/data/output/example_data.xlsx
+++ b/data/output/example_data.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,47 +422,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Kilometers from start</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Distance from track (km)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Matching Filter</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Website</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Phone</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Opening hours</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>OSM Tags</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>lat</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>lon</t>
         </is>
@@ -482,71 +475,153 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.58</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.32</v>
+        <v>4.62</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Aire camping-car de Saint Avertin</t>
+          <t>tourism=camp_site</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.onlypark.fr/aire-camping-car-de-st-avertin/</t>
+          <t>Les Acacias</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>+33 2 47 27 87 47</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>{'addr:city': 'Saint-Avertin', 'capacity': '20', 'caravans': 'yes', 'charge': '19 EUR', 'charge:conditional': '12 EUR @ (Sep-Jun)', 'contact:email': 'campingtoursvaldeloire@onlycamp.fr', 'contact:phone': '+33 2 47 27 87 47', 'contact:website': 'https://www.onlypark.fr/aire-camping-car-de-st-avertin/', 'drinking_water': 'yes', 'fee': 'yes', 'internet_access': 'wlan', 'name': 'Aire camping-car de Saint Avertin', 'network': 'Onlypark', 'operator': 'onlycamp', 'power_supply': 'yes', 'power_supply:charge': '3 EUR/4 hours', 'power_supply:fee': 'yes', 'power_supply:maxcurrent': '10', 'sanitary_dump_station': 'yes', 'sanitary_dump_station:charge': '3 EUR/20 minutes', 'sanitary_dump_station:fee': 'yes', 'shower': 'yes', 'stars': '4', 'tents': 'yes', 'toilets': 'no', 'tourism': 'camp_site', 'water_point': 'yes', 'wheelchair': 'yes'}</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>47.3708862</v>
+          <t>https://www.camping-tours.fr/</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>+33 2 47 44 08 16</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>{'addr:city': 'La Ville-aux-Dames', 'addr:postcode': '37700', 'addr:street': 'Rue Berthe Morisot', 'barrier': 'fence', 'caravans': 'yes', 'email': 'contact@camplvad.com', 'internet_access': 'yes', 'internet_access:fee': 'no', 'name': 'Les Acacias', 'phone': '+33 2 47 44 08 16', 'stars': '3', 'tents': 'yes', 'tourism': 'camp_site', 'website': 'https://www.camping-tours.fr/'}</t>
+        </is>
       </c>
       <c r="I2" t="n">
-        <v>0.7243202</v>
+        <v>47.4020858</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.7801299</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>tourism=camp_site</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Aire camping-car de Saint Avertin</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.onlypark.fr/aire-camping-car-de-st-avertin/</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>+33 2 47 27 87 47</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>{'addr:city': 'Saint-Avertin', 'capacity': '20', 'caravans': 'yes', 'charge': '19 EUR', 'charge:conditional': '12 EUR @ (Sep-Jun)', 'contact:email': 'campingtoursvaldeloire@onlycamp.fr', 'contact:phone': '+33 2 47 27 87 47', 'contact:website': 'https://www.onlypark.fr/aire-camping-car-de-st-avertin/', 'drinking_water': 'yes', 'fee': 'yes', 'internet_access': 'wlan', 'name': 'Aire camping-car de Saint Avertin', 'network': 'Onlypark', 'operator': 'onlycamp', 'power_supply': 'yes', 'power_supply:charge': '3 EUR/4 hours', 'power_supply:fee': 'yes', 'power_supply:maxcurrent': '10', 'sanitary_dump_station': 'yes', 'sanitary_dump_station:charge': '3 EUR/20 minutes', 'sanitary_dump_station:fee': 'yes', 'shower': 'yes', 'stars': '4', 'tents': 'yes', 'toilets': 'no', 'tourism': 'camp_site', 'water_point': 'yes', 'wheelchair': 'yes'}</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>47.3708862</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.7243202</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>9.91</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>tourism=camp_site</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>L'Islette - Fondettes</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>{'name': "L'Islette - Fondettes", 'tourism': 'camp_site'}</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>47.3892756</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.5959279</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>11.11</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>tourism=camp_site</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Camping La Mignardière</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>https://www.mignardiere.com/</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>+33 2 47 73 31 00</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
         <is>
           <t>{'addr:city': 'Ballan-Miré', 'addr:housenumber': '22', 'addr:postcode': '37510', 'addr:street': 'Avenue des Aubépines', 'cabins': 'yes', 'capacity:caravans': '114', 'capacity:tents': '114', 'caravans': 'yes', 'drinking_water': 'yes', 'motorhome': 'yes', 'name': 'Camping La Mignardière', 'phone': '+33 2 47 73 31 00', 'sanitary_dump_station': 'yes', 'shower': 'yes', 'stars': '4', 'tents': 'yes', 'toilets': 'yes', 'tourism': 'camp_site', 'washing_machine': 'yes', 'website': 'https://www.mignardiere.com/'}</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="I5" t="n">
         <v>47.3557614</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J5" t="n">
         <v>0.6332265</v>
       </c>
     </row>

</xml_diff>